<commit_message>
All files update from EPS v3.3.1 to v3.4.2
</commit_message>
<xml_diff>
--- a/InputData/bldgs/EoBSDwEC/Elast of Bldg Svc Demand wrt E Cost.xlsx
+++ b/InputData/bldgs/EoBSDwEC/Elast of Bldg Svc Demand wrt E Cost.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\bldgs\EoBSDwEC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shelley\Dropbox (Energy Innovation)\PC (2)\Documents\GitHub_Repositories\eps-us\InputData\bldgs\EoBSDwEC\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8ADD6E-4547-4EEB-BEF0-822A37E766B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="19425" windowHeight="11025"/>
+    <workbookView xWindow="15345" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="EoBSDwEC" sheetId="2" r:id="rId2"/>
+    <sheet name="AEO Assumptions" sheetId="3" r:id="rId2"/>
+    <sheet name="EoBSDwEC" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>EoBSDwEC Elasticity of Building Service Demand wrt Energy Cost</t>
   </si>
@@ -85,15 +87,6 @@
     <t>Rural Residential</t>
   </si>
   <si>
-    <t>Assumptions to the Annual Energy Outlook 2015</t>
-  </si>
-  <si>
-    <t>Residential Demand Module, Page 29</t>
-  </si>
-  <si>
-    <t>Commercial Demand Module, Page 42</t>
-  </si>
-  <si>
     <t>biomass</t>
   </si>
   <si>
@@ -110,12 +103,27 @@
   </si>
   <si>
     <t>Elasticity by Fuel (dimensionless)</t>
+  </si>
+  <si>
+    <t>Assumptions to the Annual Energy Outlook 2022</t>
+  </si>
+  <si>
+    <t>Residential Demand Module, Page 9</t>
+  </si>
+  <si>
+    <t>Residential Demand Module</t>
+  </si>
+  <si>
+    <t>Commercial Demand Module</t>
+  </si>
+  <si>
+    <t>Commercial Demand Module, Page 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -191,6 +199,143 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>180192</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>56784</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80972309-8111-66BD-6A2F-004C02B7BC2D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9525" y="209550"/>
+          <a:ext cx="6266667" cy="2923809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>21462</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>161814</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B337E11D-1EDF-D3C7-1972-42AAF5A0D996}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9525" y="3800475"/>
+          <a:ext cx="6107937" cy="888889"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>53975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>37337</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>50552</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56EFCB07-1318-96ED-A6C6-059F652E193A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="28575" y="4578350"/>
+          <a:ext cx="6104762" cy="1984127"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -269,6 +414,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -304,6 +466,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -479,22 +658,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="65" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -502,106 +683,139 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" s="2">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{EBAAB2B8-6D29-43EA-933D-85C23BAEEBB6}"/>
+    <hyperlink ref="B12" r:id="rId2" xr:uid="{7E80EFC1-B2EB-4244-B4A6-20E4D9863C03}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B545A04D-0C81-4573-BDE4-77F74558811D}">
+  <dimension ref="A1:A20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="2" max="3" width="19.81640625" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>19</v>
@@ -613,7 +827,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -627,7 +841,7 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -641,7 +855,7 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -655,7 +869,7 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -669,7 +883,7 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -683,9 +897,9 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B7">
         <v>-0.15</v>
@@ -697,9 +911,9 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B8">
         <v>-0.15</v>
@@ -711,9 +925,9 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B9">
         <v>-0.15</v>
@@ -725,9 +939,9 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B10">
         <v>-0.15</v>
@@ -739,9 +953,9 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B11">
         <v>-0.15</v>

</xml_diff>